<commit_message>
-updated Engine to handle more than one test case in the excel -updated keywordActions class- openurl method to create driver based upon the TestDataVariables.Browser
</commit_message>
<xml_diff>
--- a/target/classes/TestData/TestCases.xlsx
+++ b/target/classes/TestData/TestCases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="27">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Verify Whether User is able to login to TCI Dev</t>
+  </si>
+  <si>
+    <t>chrome</t>
   </si>
   <si>
     <t xml:space="preserve">http://tcidev-integration.sandbox.cloud.tibco.com
@@ -56,9 +59,6 @@
     <t>openurl</t>
   </si>
   <si>
-    <t>chrome</t>
-  </si>
-  <si>
     <t>xpath</t>
   </si>
   <si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>closebrowser</t>
+  </si>
+  <si>
+    <t>Verify Whether User is able to login to TCI Dev-2</t>
   </si>
 </sst>
 </file>
@@ -204,14 +207,10 @@
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -219,22 +218,19 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
+      <c r="G3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -242,7 +238,7 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="1">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -251,16 +247,13 @@
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -268,7 +261,7 @@
         <v>1.0</v>
       </c>
       <c r="B5" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
@@ -277,13 +270,16 @@
         <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -291,7 +287,7 @@
         <v>1.0</v>
       </c>
       <c r="B6" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
@@ -300,16 +296,13 @@
         <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -317,7 +310,7 @@
         <v>1.0</v>
       </c>
       <c r="B7" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>11</v>
@@ -326,13 +319,16 @@
         <v>15</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -340,22 +336,220 @@
         <v>1.0</v>
       </c>
       <c r="B8" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B9" s="1">
         <v>7.0</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B18" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G2"/>
+    <hyperlink r:id="rId1" ref="G3"/>
+    <hyperlink r:id="rId2" ref="G12"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-Implemented DeleteApp Method in testing class
</commit_message>
<xml_diff>
--- a/target/classes/TestData/TestCases.xlsx
+++ b/target/classes/TestData/TestCases.xlsx
@@ -12,20 +12,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="41">
+  <si>
+    <t>TestCaseID</t>
+  </si>
   <si>
     <t>Alias</t>
   </si>
   <si>
-    <t>TestCaseID</t>
+    <t>TestStepNumber</t>
   </si>
   <si>
     <t>Identifier</t>
   </si>
   <si>
+    <t>TestCaseTitle</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
     <t>Locator</t>
   </si>
   <si>
+    <t>InputLocator</t>
+  </si>
+  <si>
+    <t>InputData</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
     <t>SigninButton</t>
   </si>
   <si>
@@ -59,34 +86,7 @@
     <t>//button[@id='taLogin']</t>
   </si>
   <si>
-    <t>TestStepNumber</t>
-  </si>
-  <si>
-    <t>TestCaseTitle</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>InputLocator</t>
-  </si>
-  <si>
-    <t>InputData</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>OS</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Verify Whether User is able to login to TCI Dev</t>
+    <t>Verify Whether User is able to Create ServiceBusConnection</t>
   </si>
   <si>
     <t xml:space="preserve">http://tcidev-integration.sandbox.cloud.tibco.com
@@ -123,10 +123,19 @@
     <t>//span[@translate='TROPOS_WELCOME.ACCEPT']</t>
   </si>
   <si>
+    <t>Connector:'Microsoft Azure ServiceBus Connector',name:'AzureServiceBusConnector',description:'description',authorizationRuleName:'AuthRule',resourceURI:'ServicebusQA001',primarysecondaryKey:'eFxVfMG/8ssXCmm9BQFuEymrVnYpFvJWTxkr0nuXPQw='</t>
+  </si>
+  <si>
+    <t>createConnection</t>
+  </si>
+  <si>
+    <t>http://www.google.com</t>
+  </si>
+  <si>
+    <t>Verify Whether User is able to create Azure Storage Connection</t>
+  </si>
+  <si>
     <t>Connector:'Microsoft Azure Storage Connector',name:'AzureStorageConnector',description:'description',accountName:'tibcodevstoragev2',Select_connectionType:'Generate SAS',accessKey:'JUMuqVI6MO36YpT6zCxxAqj+3md8t2uu1X70gIbxNun1pmdWElOaeYkZog8DjJ/JIN04DuFTU0cR22hfcNQa5g==',expiryDate:'2018-12-20T21:55:07Z'</t>
-  </si>
-  <si>
-    <t>createConnection</t>
   </si>
 </sst>
 </file>
@@ -206,37 +215,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
@@ -270,10 +279,10 @@
         <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>28</v>
@@ -293,10 +302,10 @@
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>29</v>
@@ -319,10 +328,10 @@
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>28</v>
@@ -342,10 +351,10 @@
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>31</v>
@@ -368,10 +377,10 @@
         <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>28</v>
@@ -413,7 +422,7 @@
         <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>34</v>
@@ -436,7 +445,7 @@
         <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>35</v>
@@ -470,44 +479,49 @@
         <v>27</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B12" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="13">
-      <c r="A13" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="1">
         <v>2.0</v>
       </c>
       <c r="B14" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>6</v>
+        <v>39</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>27</v>
@@ -518,22 +532,19 @@
         <v>2.0</v>
       </c>
       <c r="B15" s="1">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>27</v>
@@ -544,19 +555,22 @@
         <v>2.0</v>
       </c>
       <c r="B16" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>27</v>
@@ -567,22 +581,19 @@
         <v>2.0</v>
       </c>
       <c r="B17" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>27</v>
@@ -593,19 +604,22 @@
         <v>2.0</v>
       </c>
       <c r="B18" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>27</v>
@@ -616,18 +630,19 @@
         <v>2.0</v>
       </c>
       <c r="B19" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="3" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>27</v>
@@ -638,19 +653,18 @@
         <v>2.0</v>
       </c>
       <c r="B20" s="1">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>27</v>
@@ -661,16 +675,16 @@
         <v>2.0</v>
       </c>
       <c r="B21" s="1">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>28</v>
@@ -684,261 +698,74 @@
         <v>2.0</v>
       </c>
       <c r="B22" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B23" s="1">
         <v>10.0</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H22" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B24" s="1">
-        <v>1.0</v>
+        <v>11.0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="B25" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="B26" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="B27" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="B28" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="B29" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="B30" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="B31" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="B32" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="B33" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I33" s="1" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="G2"/>
-    <hyperlink r:id="rId2" ref="G13"/>
-    <hyperlink r:id="rId3" ref="G24"/>
+    <hyperlink r:id="rId2" ref="G12"/>
+    <hyperlink r:id="rId3" ref="G14"/>
+    <hyperlink r:id="rId4" ref="G24"/>
   </hyperlinks>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -958,68 +785,68 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>